<commit_message>
added sample df merge to file list
</commit_message>
<xml_diff>
--- a/code/MAP_DAP/test_files/col_test1.xlsx
+++ b/code/MAP_DAP/test_files/col_test1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lexiescholtz/Library/CloudStorage/Dropbox/usc stuff/armani_lab/research/MAP/code/magnetophotometer/code/MAP_DAP/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57120512-0F9D-F64B-8673-F6C6BF756C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41ADEF4-1DDE-6D40-9124-9D0CF5C9D135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{898C29F9-882D-5444-B816-F3C4CFC7809E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="1" xr2:uid="{898C29F9-882D-5444-B816-F3C4CFC7809E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="samples" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +103,57 @@
   </si>
   <si>
     <t>File_name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner </t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Batch-date</t>
+  </si>
+  <si>
+    <t>Solvent</t>
+  </si>
+  <si>
+    <t>Concentration</t>
+  </si>
+  <si>
+    <t>Dilution-date</t>
+  </si>
+  <si>
+    <t>Prep-date</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>Lexie</t>
+  </si>
+  <si>
+    <t>Arlo</t>
+  </si>
+  <si>
+    <t>Iron oxide</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Dynabeads</t>
+  </si>
+  <si>
+    <t>PBS</t>
+  </si>
+  <si>
+    <t>Material</t>
   </si>
 </sst>
 </file>
@@ -133,12 +185,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -174,6 +232,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9705B542-EEE1-B643-B256-A2773E597E67}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,7 +637,9 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="G2" s="8">
         <v>3</v>
       </c>
@@ -603,7 +672,9 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="G3" s="8">
         <v>3</v>
       </c>
@@ -622,6 +693,84 @@
       </c>
       <c r="M3" s="6" t="s">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27CD9A5-E599-7040-B691-F040839579F9}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>